<commit_message>
after lot of changes
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksrag\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\001 IITM DATASCIENCE\002 Diploma\TDS\tds_project2\tds_project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="154">
   <si>
     <t>GA1.1</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>QUESTION HINT</t>
   </si>
   <si>
     <t>ANSWER</t>
@@ -924,26 +921,14 @@
     <t>Silent stories of love and loss. The necklace a treasured family heirloom was engraved with initials matching those in Edmund's diary. It hinted at a forbidden romance and a vow to protect a truth that could upend reputations and ignite fresh scandal. A creak from the chapel door startled Miranda. Peeking out, she saw a shadowed figure vanish into a corridor. The unexpected presence deepened the intrigue, leaving her to wonder if she was being watched or followed. Determined to confront the mystery, Miranda followed the elusive figure into the dim corridor. Fleeting glimpses of determination and hidden sorrow emerged, challenging her assumptions about friend and foe alike. The pursuit led her to a narrow, winding passage beneath the chapel. In the oppressive darkness, the air grew cold and heavy, and every echo of her footsteps seemed to whisper warnings of secrets best left undisturbed. In a subterranean chamber, the shadow finally halted. The figure's voice emerged from the gloom. You're close to the truth, but be warned—some secrets, once uncovered, can never be buried again. The mysterious stranger introduced himself as Victor, a former confidant of Edmund. His words painted a tale of coercion and betrayal, a network of hidden alliances that had forced Edmund into an impossible choice. Victor detailed clandestine meetings, cryptic codes, and a secret society that manipulated fate from behind the scenes. Miranda listened, each revelation tightening the knots of suspicion around her mind.From within his worn coat, Victor produced a faded journal brimming with names, dates, and enigmatic symbols.</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>return the content in the answer cell</t>
-  </si>
-  <si>
-    <t>if you are able to perform the task given in question do it, else return the content in the answer cell</t>
-  </si>
-  <si>
-    <t>formulas in Google Sheets =SUM(ARRAY_CONSTRAIN(SEQUENCE(100, 100, 4, 0), 1, 10))</t>
-  </si>
-  <si>
-    <t>compare with question hint if same formula is asked then return text in  answer cell else you perform the task</t>
-  </si>
-  <si>
-    <t>formulas in Excel
-=SUM(TAKE(SORTBY({11,8,10,8,7,3,5,12,8,5,0,4,7,12,4,15}, {10,9,13,2,11,8,16,14,7,15,5,4,6,1,3,12}), 1, 5))</t>
-  </si>
-  <si>
-    <t>if question is "Wednesdays are there in the date range 1990-07-27 to 2017-10-22?" then return content in answer cell else perform the task</t>
+    <t xml:space="preserve">formulas in Google Sheets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">formulas in Excel
+</t>
+  </si>
+  <si>
+    <t>QUESTION HINT</t>
   </si>
 </sst>
 </file>
@@ -1306,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,25 +1302,21 @@
     <col min="1" max="1" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1343,13 +1324,10 @@
         <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1357,55 +1335,43 @@
         <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="2">
         <v>40</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C6" s="2">
         <v>28</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1413,13 +1379,10 @@
         <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -1429,11 +1392,8 @@
       <c r="C8" s="2">
         <v>1421</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1441,10 +1401,10 @@
         <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1452,10 +1412,10 @@
         <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1463,10 +1423,10 @@
         <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1437,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1488,7 +1448,7 @@
         <v>25966</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1496,10 +1456,10 @@
         <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1507,10 +1467,10 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1529,7 +1489,7 @@
         <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,7 +1511,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -1562,7 +1522,7 @@
         <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,7 +1544,7 @@
         <v>73</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1595,7 +1555,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,7 +1577,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1628,7 +1588,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1599,7 @@
         <v>77</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,7 +1621,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -1672,7 +1632,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1705,7 +1665,7 @@
         <v>83</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -1716,7 +1676,7 @@
         <v>84</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -1727,7 +1687,7 @@
         <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1749,7 +1709,7 @@
         <v>87</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1760,7 +1720,7 @@
         <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1782,7 +1742,7 @@
         <v>90</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1804,7 +1764,7 @@
         <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1826,7 +1786,7 @@
         <v>94</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1848,7 +1808,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1870,7 +1830,7 @@
         <v>115</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1969,7 +1929,7 @@
         <v>105</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>